<commit_message>
Data for ANN is added
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>S. No</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Random Forest (100 Trees)</t>
+  </si>
+  <si>
+    <t>Deep Learning Models</t>
+  </si>
+  <si>
+    <t>ANN</t>
   </si>
 </sst>
 </file>
@@ -391,16 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
@@ -434,16 +440,16 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0.375</v>
+        <v>0.49</v>
       </c>
       <c r="D2">
         <v>0.38800000000000001</v>
       </c>
       <c r="E2">
-        <v>0.48</v>
+        <v>0.626</v>
       </c>
       <c r="F2">
-        <v>0.43</v>
+        <v>0.47899999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -454,16 +460,16 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>0.67500000000000004</v>
+        <v>0.68</v>
       </c>
       <c r="D3">
         <v>0.79300000000000004</v>
       </c>
       <c r="E3">
-        <v>0.70499999999999996</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="F3">
-        <v>0.747</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -474,16 +480,16 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.83499999999999996</v>
+        <v>0.64</v>
       </c>
       <c r="D4">
-        <v>0.9</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="E4">
-        <v>0.83799999999999997</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="F4">
-        <v>0.86799999999999999</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -494,16 +500,16 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0.56999999999999995</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="D5">
         <v>0.68500000000000005</v>
       </c>
       <c r="E5">
-        <v>0.63300000000000001</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="F5">
-        <v>0.65800000000000003</v>
+        <v>0.70599999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -514,16 +520,16 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>0.8</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="D6">
         <v>0.9</v>
       </c>
       <c r="E6">
-        <v>0.79500000000000004</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="F6">
-        <v>0.84399999999999997</v>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -534,16 +540,16 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>0.55500000000000005</v>
+        <v>0.63</v>
       </c>
       <c r="D7">
         <v>0.65200000000000002</v>
       </c>
       <c r="E7">
-        <v>0.626</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="F7">
-        <v>0.63900000000000001</v>
+        <v>0.68100000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,16 +560,41 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>0.75</v>
+        <v>0.66</v>
       </c>
       <c r="D8">
         <v>0.85899999999999999</v>
       </c>
       <c r="E8">
-        <v>0.75900000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="F8">
-        <v>0.80600000000000005</v>
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="D11">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="E11">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="F11">
+        <v>0.66300000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ANN and XGBoost Added
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>S. No</t>
   </si>
@@ -63,7 +63,16 @@
     <t>Deep Learning Models</t>
   </si>
   <si>
-    <t>ANN</t>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>Miscellaneous Model</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>ANN (1st layer = 10, 2nd Layer = 6)</t>
   </si>
 </sst>
 </file>
@@ -397,16 +406,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
     <col min="3" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
@@ -440,16 +449,16 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0.49</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="D2">
-        <v>0.38800000000000001</v>
+        <v>0.38</v>
       </c>
       <c r="E2">
-        <v>0.626</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="F2">
-        <v>0.47899999999999998</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -460,16 +469,16 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>0.68</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="D3">
-        <v>0.79300000000000004</v>
+        <v>0.81299999999999994</v>
       </c>
       <c r="E3">
-        <v>0.71099999999999997</v>
+        <v>0.73</v>
       </c>
       <c r="F3">
-        <v>0.75</v>
+        <v>0.76900000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,16 +489,16 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="D4">
-        <v>0.89200000000000002</v>
+        <v>0.86</v>
       </c>
       <c r="E4">
-        <v>0.64600000000000002</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="F4">
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -500,16 +509,16 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0.65500000000000003</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="D5">
-        <v>0.68500000000000005</v>
+        <v>0.72</v>
       </c>
       <c r="E5">
-        <v>0.72799999999999998</v>
+        <v>0.755</v>
       </c>
       <c r="F5">
-        <v>0.70599999999999996</v>
+        <v>0.73699999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -520,16 +529,16 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>0.68500000000000005</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="D6">
-        <v>0.9</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="E6">
-        <v>0.68100000000000005</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="F6">
-        <v>0.77500000000000002</v>
+        <v>0.78800000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -540,16 +549,16 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>0.63</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="D7">
-        <v>0.65200000000000002</v>
+        <v>0.66</v>
       </c>
       <c r="E7">
-        <v>0.71099999999999997</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="F7">
-        <v>0.68100000000000005</v>
+        <v>0.67300000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -560,16 +569,16 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>0.66</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="D8">
-        <v>0.85899999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="E8">
-        <v>0.67</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="F8">
-        <v>0.753</v>
+        <v>0.76800000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -582,19 +591,52 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>0.48</v>
+      </c>
+      <c r="D11">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="F11">
+        <v>0.47099999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
-        <v>0.60499999999999998</v>
-      </c>
-      <c r="D11">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="E11">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="F11">
-        <v>0.66300000000000003</v>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="D15">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="E15">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F15">
+        <v>0.78400000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CNN and CatBoost Added
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>S. No</t>
   </si>
@@ -63,16 +63,19 @@
     <t>Deep Learning Models</t>
   </si>
   <si>
-    <t>CNN</t>
-  </si>
-  <si>
     <t>Miscellaneous Model</t>
   </si>
   <si>
     <t>XGBoost</t>
   </si>
   <si>
-    <t>ANN (1st layer = 10, 2nd Layer = 6)</t>
+    <t xml:space="preserve">CNN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANN </t>
+  </si>
+  <si>
+    <t>CatBoost</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,12 +614,24 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="E12">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="F12">
+        <v>0.67800000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>0.70799999999999996</v>
@@ -637,6 +652,26 @@
       </c>
       <c r="F15">
         <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="D16">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="E16">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F16">
+        <v>0.77100000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>